<commit_message>
update obstaion most year 2019
</commit_message>
<xml_diff>
--- a/data-raw/data-tidy/hack-tianyan/hub/match-tianyan-tot7-2022-08-17.xlsx
+++ b/data-raw/data-tidy/hack-tianyan/hub/match-tianyan-tot7-2022-08-17.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\techme\data-raw\data-tidy\hack-tianyan\hub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037B9DCB-BCA9-4E4D-943F-A64E858951DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2209BC-6944-49D6-B56E-6FD5A0C50145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9892" yWindow="8258" windowWidth="24495" windowHeight="15674" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="3090" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -507,7 +507,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>